<commit_message>
se arreglan: - Recording BuscarGrupos.rxrec, Se agrega recording Selecciona_CodigoAgente.rxrec - Se mejora el recording NuevaPolizaAP.rxrec en la parte del wait for not exist del item MetodoDePago - Se mejoran los recording de CantCuotasSi.rxrec y Cant_Cuotas.rxrec se agregaron wait for not exit del item OPCION_PAGOCUOTAS
</commit_message>
<xml_diff>
--- a/Sura/DataSource - Emision AP - Nomina Parte 2.xlsx
+++ b/Sura/DataSource - Emision AP - Nomina Parte 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Sura\Sura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71F660C5-BC66-4B45-BD9E-F501C7D1B135}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0194C722-06DE-457B-9A21-C65B3919FB81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,7 +54,7 @@
     <t>silverarrow</t>
   </si>
   <si>
-    <t>2240451788</t>
+    <t>7635954411</t>
   </si>
 </sst>
 </file>
@@ -390,7 +390,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>